<commit_message>
more updates for functional tests
</commit_message>
<xml_diff>
--- a/aat/src/aat/resources/CCD_BEFTA_JURISDICTION3.xlsx
+++ b/aat/src/aat/resources/CCD_BEFTA_JURISDICTION3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccabaker/HMCTS/Reform/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veeresha/hmcts/git/ccd-definition-store-api/aat/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8082B7-E97F-3B44-9D37-D293B33733AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997C5752-30D4-1941-A169-39DDA9996126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3868" uniqueCount="341">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1051,6 +1051,39 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>BEFTA_CASETYPE_3_4</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>Demo Case BEFTA CASETYPE 3 4</t>
+  </si>
+  <si>
+    <t>BEFTA_JURISDICTION_4</t>
+  </si>
+  <si>
+    <t>MetaLabelField</t>
+  </si>
+  <si>
+    <t>A 'Label' field with last modified date as interpolation $[LAST_STATE_MODIFIED_DATE]</t>
+  </si>
+  <si>
+    <t>[LAST_STATE_MODIFIED_DATE]</t>
+  </si>
+  <si>
+    <t>Last State Modified Date</t>
+  </si>
+  <si>
+    <t>`Number` field</t>
+  </si>
+  <si>
+    <t>`YesOrNo` field</t>
   </si>
 </sst>
 </file>
@@ -1459,7 +1492,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1578,6 +1611,7 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2006,10 +2040,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="A10" sqref="A10:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2182,31 +2216,90 @@
         <v>2</v>
       </c>
     </row>
+    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>337</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="F11" s="86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>42736</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>339</v>
+      </c>
+      <c r="F12" s="86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>340</v>
+      </c>
+      <c r="F13" s="86">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0900-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F10" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0900-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A13" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
-          <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$35</xm:f>
-          </x14:formula1>
-          <xm:sqref>D4:D9</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -2216,10 +2309,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2339,15 +2432,51 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="F8" s="21">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F6" xr:uid="{00000000-0002-0000-0A00-000002000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F8" xr:uid="{00000000-0002-0000-0A00-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -2373,10 +2502,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2549,15 +2678,84 @@
         <v>2</v>
       </c>
     </row>
+    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>337</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="F11" s="86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>42736</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>339</v>
+      </c>
+      <c r="F12" s="86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>340</v>
+      </c>
+      <c r="F13" s="86">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F9" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F10" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A9" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A13" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B9" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B10" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -2583,10 +2781,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54:H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4024,15 +4222,150 @@
         <v>1</v>
       </c>
     </row>
+    <row r="54" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B54" s="27"/>
+      <c r="C54" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E54" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="G54" s="28">
+        <v>1</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="I54" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B55" s="27"/>
+      <c r="C55" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E55" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="G55" s="28">
+        <v>1</v>
+      </c>
+      <c r="H55" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="I55" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B56" s="27"/>
+      <c r="C56" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E56" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="G56" s="28">
+        <v>1</v>
+      </c>
+      <c r="H56" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="I56" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B57" s="27"/>
+      <c r="C57" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E57" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="G57" s="28">
+        <v>1</v>
+      </c>
+      <c r="H57" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="I57" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B58" s="27"/>
+      <c r="C58" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E58" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="G58" s="28">
+        <v>2</v>
+      </c>
+      <c r="H58" s="41" t="s">
+        <v>258</v>
+      </c>
+      <c r="I58" s="28">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G53 I4:I53" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="I4:I58 G4:G58" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A53" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A58" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B53" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B58" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -4177,10 +4510,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4282,6 +4615,21 @@
         <v>58</v>
       </c>
     </row>
+    <row r="7" spans="1:5" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4295,10 +4643,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4526,6 +4874,60 @@
         <v>123</v>
       </c>
     </row>
+    <row r="13" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>280</v>
+      </c>
+      <c r="F13" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="58">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F15" s="73" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4539,10 +4941,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F24"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67:D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5692,6 +6094,74 @@
         <v>329</v>
       </c>
     </row>
+    <row r="67" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D67" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D68" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D69" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D70" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5705,10 +6175,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6619,6 +7089,91 @@
         <v>281</v>
       </c>
       <c r="F52" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F53" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F55" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D57" s="41" t="s">
+        <v>258</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F57" s="24" t="s">
         <v>123</v>
       </c>
     </row>
@@ -6637,7 +7192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="144" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="144" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -6839,10 +7394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6996,12 +7551,33 @@
         <v>116</v>
       </c>
     </row>
+    <row r="7" spans="1:9" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>334</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" xWindow="279" yWindow="381" count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations xWindow="279" yWindow="381" count="2">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A7" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B7" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -7017,10 +7593,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8606,12 +9182,155 @@
         <v>116</v>
       </c>
     </row>
+    <row r="54" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F55" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J55" s="28"/>
+      <c r="K55" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B56" s="13"/>
+      <c r="C56" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="E56" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B57" s="13"/>
+      <c r="C57" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="G57" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B58" s="13"/>
+      <c r="C58" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D58" s="41" t="s">
+        <v>258</v>
+      </c>
+      <c r="E58" s="41" t="s">
+        <v>259</v>
+      </c>
+      <c r="F58" s="41" t="s">
+        <v>260</v>
+      </c>
+      <c r="G58" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="H58" s="41"/>
+      <c r="I58" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A53" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A58" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B53" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B58" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -9163,10 +9882,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9404,15 +10123,72 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G12" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G15" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A12" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A15" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B12" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B15" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -9428,10 +10204,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D25"/>
+    <sheetView topLeftCell="A55" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70:D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11910,15 +12686,161 @@
         <v>72</v>
       </c>
     </row>
+    <row r="70" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B70" s="13"/>
+      <c r="C70" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D70" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E70" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="F70" s="28"/>
+      <c r="G70" s="28">
+        <v>1</v>
+      </c>
+      <c r="H70" s="28"/>
+      <c r="I70" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="J70" s="29"/>
+      <c r="K70" s="29"/>
+      <c r="L70" s="29"/>
+      <c r="M70" s="29"/>
+      <c r="N70" s="29"/>
+      <c r="O70" s="29"/>
+      <c r="P70" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q70" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D71" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E71" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28">
+        <v>2</v>
+      </c>
+      <c r="H71" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="I71" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="J71" s="29"/>
+      <c r="K71" s="29"/>
+      <c r="L71" s="29"/>
+      <c r="M71" s="29"/>
+      <c r="N71" s="29"/>
+      <c r="O71" s="29"/>
+      <c r="P71" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q71" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B72" s="13"/>
+      <c r="C72" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D72" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E72" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="F72" s="28"/>
+      <c r="G72" s="28">
+        <v>3</v>
+      </c>
+      <c r="H72" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="I72" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="J72" s="29"/>
+      <c r="K72" s="29"/>
+      <c r="L72" s="29"/>
+      <c r="M72" s="29"/>
+      <c r="N72" s="29"/>
+      <c r="O72" s="29"/>
+      <c r="P72" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q72" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B73" s="13"/>
+      <c r="C73" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D73" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="E73" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28">
+        <v>4</v>
+      </c>
+      <c r="H73" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="I73" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="J73" s="29"/>
+      <c r="K73" s="29"/>
+      <c r="L73" s="29"/>
+      <c r="M73" s="29"/>
+      <c r="N73" s="29"/>
+      <c r="O73" s="29"/>
+      <c r="P73" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q73" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G69" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G73" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9 B26:B31 B48:B53" xr:uid="{00000000-0002-0000-0600-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that is after LiveFrom date" sqref="B4:B9 B26:B31 B48:B53 B70:B73" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A69" xr:uid="{00000000-0002-0000-0600-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="A4:A73" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
   </dataValidations>
@@ -11934,10 +12856,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O184"/>
+  <dimension ref="A1:O200"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107:XFD123"/>
+    <sheetView topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="E185" sqref="E185:E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18718,12 +19640,604 @@
         <v>25</v>
       </c>
     </row>
+    <row r="185" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A185" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B185" s="13"/>
+      <c r="C185" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D185" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E185" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F185" s="28">
+        <v>1</v>
+      </c>
+      <c r="G185" s="28"/>
+      <c r="H185" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I185" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J185" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K185" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L185" s="14">
+        <v>1</v>
+      </c>
+      <c r="O185" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A186" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B186" s="13"/>
+      <c r="C186" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D186" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E186" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="F186" s="28">
+        <v>2</v>
+      </c>
+      <c r="G186" s="28"/>
+      <c r="H186" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I186" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J186" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K186" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L186" s="14">
+        <v>1</v>
+      </c>
+      <c r="O186" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A187" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B187" s="13"/>
+      <c r="C187" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D187" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E187" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F187" s="28">
+        <v>3</v>
+      </c>
+      <c r="G187" s="28"/>
+      <c r="H187" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I187" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J187" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K187" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L187" s="14">
+        <v>1</v>
+      </c>
+      <c r="O187" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A188" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B188" s="13"/>
+      <c r="C188" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D188" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E188" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F188" s="28">
+        <v>4</v>
+      </c>
+      <c r="G188" s="28"/>
+      <c r="H188" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I188" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J188" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K188" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L188" s="14">
+        <v>1</v>
+      </c>
+      <c r="O188" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A189" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B189" s="13"/>
+      <c r="C189" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D189" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E189" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F189" s="28">
+        <v>1</v>
+      </c>
+      <c r="G189" s="28"/>
+      <c r="H189" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I189" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J189" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K189" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L189" s="14">
+        <v>1</v>
+      </c>
+      <c r="O189" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A190" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B190" s="13"/>
+      <c r="C190" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D190" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E190" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="F190" s="28">
+        <v>2</v>
+      </c>
+      <c r="G190" s="28"/>
+      <c r="H190" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I190" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J190" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K190" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L190" s="14">
+        <v>1</v>
+      </c>
+      <c r="O190" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A191" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B191" s="13"/>
+      <c r="C191" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D191" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E191" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F191" s="28">
+        <v>3</v>
+      </c>
+      <c r="G191" s="28"/>
+      <c r="H191" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I191" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J191" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K191" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L191" s="14">
+        <v>1</v>
+      </c>
+      <c r="O191" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A192" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B192" s="13"/>
+      <c r="C192" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D192" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E192" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F192" s="28">
+        <v>4</v>
+      </c>
+      <c r="G192" s="28"/>
+      <c r="H192" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I192" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J192" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K192" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L192" s="14">
+        <v>1</v>
+      </c>
+      <c r="O192" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A193" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B193" s="13"/>
+      <c r="C193" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D193" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E193" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F193" s="28">
+        <v>1</v>
+      </c>
+      <c r="G193" s="28"/>
+      <c r="H193" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I193" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J193" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K193" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L193" s="14">
+        <v>1</v>
+      </c>
+      <c r="O193" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A194" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B194" s="13"/>
+      <c r="C194" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D194" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E194" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="F194" s="28">
+        <v>2</v>
+      </c>
+      <c r="G194" s="28"/>
+      <c r="H194" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I194" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J194" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K194" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L194" s="14">
+        <v>1</v>
+      </c>
+      <c r="O194" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A195" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B195" s="13"/>
+      <c r="C195" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D195" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E195" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F195" s="28">
+        <v>3</v>
+      </c>
+      <c r="G195" s="28"/>
+      <c r="H195" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I195" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J195" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K195" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L195" s="14">
+        <v>1</v>
+      </c>
+      <c r="O195" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A196" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B196" s="13"/>
+      <c r="C196" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D196" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="E196" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F196" s="28">
+        <v>4</v>
+      </c>
+      <c r="G196" s="28"/>
+      <c r="H196" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I196" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J196" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K196" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L196" s="14">
+        <v>1</v>
+      </c>
+      <c r="O196" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A197" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B197" s="13"/>
+      <c r="C197" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D197" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="E197" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F197" s="28">
+        <v>1</v>
+      </c>
+      <c r="G197" s="28"/>
+      <c r="H197" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I197" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J197" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K197" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L197" s="14">
+        <v>1</v>
+      </c>
+      <c r="O197" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A198" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B198" s="13"/>
+      <c r="C198" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D198" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="E198" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="F198" s="28">
+        <v>2</v>
+      </c>
+      <c r="G198" s="28"/>
+      <c r="H198" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I198" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J198" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K198" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L198" s="14">
+        <v>1</v>
+      </c>
+      <c r="O198" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A199" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B199" s="13"/>
+      <c r="C199" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D199" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="E199" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F199" s="28">
+        <v>3</v>
+      </c>
+      <c r="G199" s="28"/>
+      <c r="H199" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I199" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J199" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K199" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L199" s="14">
+        <v>1</v>
+      </c>
+      <c r="O199" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A200" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B200" s="13"/>
+      <c r="C200" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D200" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="E200" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F200" s="28">
+        <v>4</v>
+      </c>
+      <c r="G200" s="28"/>
+      <c r="H200" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I200" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="J200" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="K200" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="L200" s="14">
+        <v>1</v>
+      </c>
+      <c r="O200" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A184" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A200" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B184" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B200" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -18739,10 +20253,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18861,31 +20375,57 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="F8" s="21">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F6" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F8" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A6" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A8" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B6" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date that is after 'LiveFrom' date" sqref="B4:B8" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
-          <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$35</xm:f>
-          </x14:formula1>
-          <xm:sqref>D4:D6</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>

</xml_diff>

<commit_message>
added sort order data for func. tests
</commit_message>
<xml_diff>
--- a/aat/src/aat/resources/CCD_BEFTA_JURISDICTION3.xlsx
+++ b/aat/src/aat/resources/CCD_BEFTA_JURISDICTION3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veeresha/hmcts/git/ccd-definition-store-api/aat/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997C5752-30D4-1941-A169-39DDA9996126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA52250F-2539-9549-A63A-F85AE7F03A84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="940" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3868" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3872" uniqueCount="344">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1071,9 +1071,6 @@
     <t>MetaLabelField</t>
   </si>
   <si>
-    <t>A 'Label' field with last modified date as interpolation $[LAST_STATE_MODIFIED_DATE]</t>
-  </si>
-  <si>
     <t>[LAST_STATE_MODIFIED_DATE]</t>
   </si>
   <si>
@@ -1084,6 +1081,18 @@
   </si>
   <si>
     <t>`YesOrNo` field</t>
+  </si>
+  <si>
+    <t>A 'Label' field with last modified date as interpolation ${[LAST_STATE_MODIFIED_DATE]}</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>1:ASC</t>
+  </si>
+  <si>
+    <t>1:DESC</t>
   </si>
 </sst>
 </file>
@@ -1492,7 +1501,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1612,6 +1621,7 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2040,10 +2050,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2056,7 +2066,7 @@
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -2072,7 +2082,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="29" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="29" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30" t="s">
@@ -2088,7 +2098,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2107,8 +2117,11 @@
       <c r="F3" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="87" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>42736</v>
       </c>
@@ -2126,7 +2139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>42736</v>
       </c>
@@ -2144,7 +2157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>42736</v>
       </c>
@@ -2162,7 +2175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>42736</v>
       </c>
@@ -2180,7 +2193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23">
         <v>42736</v>
       </c>
@@ -2198,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23">
         <v>42736</v>
       </c>
@@ -2216,7 +2229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23">
         <v>42736</v>
       </c>
@@ -2225,16 +2238,19 @@
         <v>330</v>
       </c>
       <c r="D10" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>337</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>338</v>
-      </c>
       <c r="F10" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G10" s="86" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23">
         <v>42736</v>
       </c>
@@ -2251,7 +2267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23">
         <v>42736</v>
       </c>
@@ -2262,13 +2278,13 @@
         <v>135</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F12" s="86">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23">
         <v>42736</v>
       </c>
@@ -2279,14 +2295,14 @@
         <v>137</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F13" s="86">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="F4:F10" xr:uid="{00000000-0002-0000-0900-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
@@ -2459,10 +2475,10 @@
         <v>330</v>
       </c>
       <c r="D8" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>337</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>338</v>
       </c>
       <c r="F8" s="21">
         <v>2</v>
@@ -2502,10 +2518,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2516,9 +2532,10 @@
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -2534,7 +2551,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="29" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="29" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="33"/>
       <c r="B2" s="33"/>
       <c r="C2" s="30" t="s">
@@ -2550,7 +2567,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2569,8 +2586,11 @@
       <c r="F3" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="87" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>42736</v>
       </c>
@@ -2588,7 +2608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>42736</v>
       </c>
@@ -2606,7 +2626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>42736</v>
       </c>
@@ -2624,7 +2644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>42736</v>
       </c>
@@ -2642,7 +2662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23">
         <v>42736</v>
       </c>
@@ -2660,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23">
         <v>42736</v>
       </c>
@@ -2678,7 +2698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23">
         <v>42736</v>
       </c>
@@ -2687,16 +2707,19 @@
         <v>330</v>
       </c>
       <c r="D10" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>337</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>338</v>
-      </c>
       <c r="F10" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G10" s="86" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23">
         <v>42736</v>
       </c>
@@ -2713,7 +2736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23">
         <v>42736</v>
       </c>
@@ -2724,13 +2747,13 @@
         <v>135</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F12" s="86">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23">
         <v>42736</v>
       </c>
@@ -2741,7 +2764,7 @@
         <v>137</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F13" s="86">
         <v>4</v>
@@ -2783,8 +2806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54:H57"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4384,7 +4407,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7192,7 +7215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="144" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="144" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -7396,7 +7419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -7595,8 +7618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54:D58"/>
+    <sheetView topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9252,7 +9275,7 @@
         <v>335</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="F56" s="28"/>
       <c r="G56" s="28" t="s">
@@ -10206,8 +10229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70:D73"/>
+    <sheetView topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12858,8 +12881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O200"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="E185" sqref="E185:E188"/>
+    <sheetView topLeftCell="C169" workbookViewId="0">
+      <selection activeCell="K190" sqref="K190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20402,10 +20425,10 @@
         <v>330</v>
       </c>
       <c r="D8" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>337</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>338</v>
       </c>
       <c r="F8" s="21">
         <v>2</v>

</xml_diff>

<commit_message>
updated per review comments
</commit_message>
<xml_diff>
--- a/aat/src/aat/resources/CCD_BEFTA_JURISDICTION3.xlsx
+++ b/aat/src/aat/resources/CCD_BEFTA_JURISDICTION3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veeresha/hmcts/git/ccd-definition-store-api/aat/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA52250F-2539-9549-A63A-F85AE7F03A84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677F1DA8-3872-4342-B7A1-C7F04BFCDD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="940" windowWidth="28800" windowHeight="16420" tabRatio="823" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="28800" windowHeight="16420" tabRatio="823" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,18 @@
     <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
     <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -46,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3872" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3872" uniqueCount="343">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1063,9 +1071,6 @@
   </si>
   <si>
     <t>Demo Case BEFTA CASETYPE 3 4</t>
-  </si>
-  <si>
-    <t>BEFTA_JURISDICTION_4</t>
   </si>
   <si>
     <t>MetaLabelField</t>
@@ -2118,7 +2123,7 @@
         <v>36</v>
       </c>
       <c r="G3" s="87" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2238,16 +2243,16 @@
         <v>330</v>
       </c>
       <c r="D10" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>336</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>337</v>
-      </c>
       <c r="F10" s="21">
         <v>1</v>
       </c>
       <c r="G10" s="86" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2278,7 +2283,7 @@
         <v>135</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F12" s="86">
         <v>3</v>
@@ -2295,7 +2300,7 @@
         <v>137</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F13" s="86">
         <v>4</v>
@@ -2475,10 +2480,10 @@
         <v>330</v>
       </c>
       <c r="D8" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>336</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>337</v>
       </c>
       <c r="F8" s="21">
         <v>2</v>
@@ -2520,7 +2525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -2587,7 +2592,7 @@
         <v>36</v>
       </c>
       <c r="G3" s="87" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2707,16 +2712,16 @@
         <v>330</v>
       </c>
       <c r="D10" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>336</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>337</v>
-      </c>
       <c r="F10" s="21">
         <v>1</v>
       </c>
       <c r="G10" s="86" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2747,7 +2752,7 @@
         <v>135</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F12" s="86">
         <v>3</v>
@@ -2764,7 +2769,7 @@
         <v>137</v>
       </c>
       <c r="E13" s="86" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F13" s="86">
         <v>4</v>
@@ -4320,7 +4325,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I56" s="28">
         <v>3</v>
@@ -7157,7 +7162,7 @@
         <v>330</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E55" s="14" t="s">
         <v>280</v>
@@ -7419,8 +7424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7589,7 +7594,7 @@
         <v>333</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>334</v>
+        <v>272</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>116</v>
@@ -9272,10 +9277,10 @@
         <v>330</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F56" s="28"/>
       <c r="G56" s="28" t="s">
@@ -19712,7 +19717,7 @@
         <v>188</v>
       </c>
       <c r="E186" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F186" s="28">
         <v>2</v>
@@ -19860,7 +19865,7 @@
         <v>196</v>
       </c>
       <c r="E190" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F190" s="28">
         <v>2</v>
@@ -20008,7 +20013,7 @@
         <v>194</v>
       </c>
       <c r="E194" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F194" s="28">
         <v>2</v>
@@ -20156,7 +20161,7 @@
         <v>332</v>
       </c>
       <c r="E198" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F198" s="28">
         <v>2</v>
@@ -20425,10 +20430,10 @@
         <v>330</v>
       </c>
       <c r="D8" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>336</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>337</v>
       </c>
       <c r="F8" s="21">
         <v>2</v>

</xml_diff>